<commit_message>
Balance hero - Enemy - gun
</commit_message>
<xml_diff>
--- a/Data/GunLevelConfig.xlsx
+++ b/Data/GunLevelConfig.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="13460" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Level</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>GoldUpgrade</t>
+  </si>
+  <si>
+    <t>!ATK</t>
+  </si>
+  <si>
+    <t>!Tỷ lệ upgrade sau 5 lv</t>
+  </si>
+  <si>
+    <t>!Tỷ lệ nhân</t>
   </si>
 </sst>
 </file>
@@ -98,8 +107,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -114,17 +133,27 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,15 +483,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,25 +502,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -496,25 +537,34 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
@@ -522,48 +572,1113 @@
         <v>50</v>
       </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>ROUND(POWER(C3, 1 / 5), 2)</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>B3 *E3</f>
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>150</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <f>A3 +1</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>ROUND(B3*D4, 0)</f>
+        <v>58</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D27" si="0">ROUND(POWER(C4, 1 / 5), 2)</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E4">
+        <f>E3</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F27" si="1">B4 *E4</f>
+        <v>58</v>
+      </c>
+      <c r="G4">
+        <f>G3</f>
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <f>H3</f>
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <f>I3</f>
+        <v>150</v>
+      </c>
+      <c r="J4">
+        <f>J3</f>
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f>K3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <f t="shared" ref="A5:A26" si="2">A4 +1</f>
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>150</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>55</v>
-      </c>
-      <c r="C4">
+      <c r="B5">
+        <f t="shared" ref="B5:B27" si="3">ROUND(B4*D5, 0)</f>
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E27" si="4">E4</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G27" si="5">G4</f>
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H27" si="6">H4</f>
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I27" si="7">I4</f>
+        <v>150</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J27" si="8">J4</f>
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K27" si="9">K4</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>160</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1200</v>
+      <c r="B6">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="3"/>
+        <v>102</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="3"/>
+        <v>117</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="3"/>
+        <v>155</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>155</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="3"/>
+        <v>178</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>178</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="3"/>
+        <v>205</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>205</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>236</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="3"/>
+        <v>271</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>271</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="3"/>
+        <v>312</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>312</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="3"/>
+        <v>359</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>359</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="3"/>
+        <v>413</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="3"/>
+        <v>475</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>475</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="3"/>
+        <v>546</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>546</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="3"/>
+        <v>628</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>628</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="3"/>
+        <v>722</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>722</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="3"/>
+        <v>830</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>830</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="3"/>
+        <v>955</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>955</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="3"/>
+        <v>1098</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1098</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="3"/>
+        <v>1263</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1263</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <f>A26 +1</f>
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="3"/>
+        <v>1452</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>1452</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="9"/>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>